<commit_message>
parse_metadata working w tests
</commit_message>
<xml_diff>
--- a/kbs/kb_min.xlsx
+++ b/kbs/kb_min.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="375" windowWidth="23250" windowHeight="12090" tabRatio="1000"/>
+    <workbookView xWindow="-105" yWindow="375" windowWidth="23250" windowHeight="12090" tabRatio="1000" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="KB" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="RNAs" sheetId="9" r:id="rId9"/>
     <sheet name="Proteins" sheetId="10" r:id="rId10"/>
     <sheet name="Complexes" sheetId="11" r:id="rId11"/>
-    <sheet name="Species properties" sheetId="12" r:id="rId12"/>
+    <sheet name="SpeciesType properties" sheetId="12" r:id="rId12"/>
     <sheet name="Concentrations" sheetId="13" r:id="rId13"/>
     <sheet name="Observables" sheetId="14" r:id="rId14"/>
     <sheet name="Reactions" sheetId="15" r:id="rId15"/>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="212">
   <si>
     <t>Id</t>
   </si>
@@ -382,27 +382,9 @@
     <t>Formation process</t>
   </si>
   <si>
-    <t>Structure</t>
-  </si>
-  <si>
-    <t>Half life</t>
-  </si>
-  <si>
-    <t>Half life units</t>
-  </si>
-  <si>
-    <t>Domains</t>
-  </si>
-  <si>
-    <t>Prosthetic groups</t>
-  </si>
-  <si>
     <t>min</t>
   </si>
   <si>
-    <t>{"source": "Pfam", "xid": "PF00712.14", "label": "DNA_pol3_beta", "start_position": 1, "end_position": 120, "score": 51.4}, {"source": "Pfam", "xid": "PF03836.10", "label": "RasGAP_C", "start_position": 51, "end_position": 116, "score": 14.6}, {"source": "Pfam", "xid": "PF02767.11", "label": "DNA_pol3_beta_2", "start_position": 136, "end_position": 255, "score": 23.1}, {"source": "Pfam", "xid": "PF02768.10", "label": "DNA_pol3_beta_3", "start_position": 259, "end_position": 379, "score": 105.6}, {"source": "NCBI-CD", "xid": "cd00140", "label": "beta_clamp", "start_position": 23, "end_position": 380, "score": 224.312}, {"source": "NCBI-CD", "xid": "cl17512", "label": "beta_clamp superfamily", "start_position": 23, "end_position": 380, "score": 224.312}, {"source": "NCBI-CD", "xid": "smart00480", "label": "POL3Bc", "start_position": 23, "end_position": 377, "score": 316.842}</t>
-  </si>
-  <si>
     <t>EVI1111</t>
   </si>
   <si>
@@ -737,6 +719,12 @@
   </si>
   <si>
     <t>test_kb</t>
+  </si>
+  <si>
+    <t>Species type</t>
+  </si>
+  <si>
+    <t>structure</t>
   </si>
 </sst>
 </file>
@@ -1676,7 +1664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -1695,7 +1683,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1703,7 +1691,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1896,7 +1884,7 @@
         <v>93</v>
       </c>
       <c r="R2" s="125" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="S2" s="123" t="s">
         <v>41</v>
@@ -1996,10 +1984,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2007,98 +1995,119 @@
     <col min="1" max="1" width="20.7109375" style="65" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" style="65" customWidth="1"/>
     <col min="3" max="4" width="15.7109375" style="3" customWidth="1"/>
-    <col min="5" max="6" width="15.7109375" style="65" customWidth="1"/>
-    <col min="7" max="9" width="20.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" style="65" customWidth="1"/>
-    <col min="11" max="21" width="9.140625" style="65" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="65"/>
+    <col min="5" max="5" width="15.7109375" style="65" customWidth="1"/>
+    <col min="6" max="8" width="20.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="65" customWidth="1"/>
+    <col min="10" max="20" width="9.140625" style="65" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="65"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="B1" s="33" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="129" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="129" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="144" t="s">
+        <v>211</v>
+      </c>
+      <c r="D2" s="129" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="129" t="s">
+        <v>125</v>
+      </c>
+      <c r="I2" s="129"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="129" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="129" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="144" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" s="129">
+        <v>4.8828698208797903</v>
+      </c>
+      <c r="E3" s="129" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="F3" s="129" t="s">
+        <v>100</v>
+      </c>
+      <c r="I3" s="129"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="129" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="129" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="144" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="129">
+        <v>992.98255190377824</v>
+      </c>
+      <c r="E4" s="129" t="s">
+        <v>97</v>
+      </c>
+      <c r="F4" s="129" t="s">
         <v>98</v>
       </c>
-      <c r="D1" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" s="33" t="s">
-        <v>100</v>
-      </c>
-      <c r="F1" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="102" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" s="102" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102" t="s">
-        <v>102</v>
-      </c>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-    </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="107" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" s="108"/>
-      <c r="C3" s="107">
-        <v>4.8828698208797903</v>
-      </c>
-      <c r="D3" s="107" t="s">
-        <v>102</v>
-      </c>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="128" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" s="129"/>
-      <c r="C4" s="128">
-        <v>992.98255190377824</v>
-      </c>
-      <c r="D4" s="128" t="s">
-        <v>102</v>
-      </c>
-      <c r="E4" s="128" t="s">
-        <v>103</v>
-      </c>
-      <c r="F4" s="128"/>
-      <c r="G4" s="128" t="s">
-        <v>104</v>
-      </c>
+      <c r="I4" s="129"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="D15" s="102"/>
+      <c r="E15" s="103"/>
+    </row>
+    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="B16" s="108"/>
+      <c r="D16" s="107"/>
+      <c r="E16" s="107"/>
+    </row>
+    <row r="17" spans="2:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="B17" s="129"/>
+      <c r="D17" s="128"/>
+      <c r="E17" s="128"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2125,13 +2134,13 @@
         <v>94</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E1" s="33" t="s">
         <v>36</v>
@@ -2151,16 +2160,16 @@
         <v>69</v>
       </c>
       <c r="B2" s="99" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C2" s="99">
         <v>4.2500000000000003E-2</v>
       </c>
       <c r="D2" s="99" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E2" s="99" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -2168,16 +2177,16 @@
         <v>77</v>
       </c>
       <c r="B3" s="111" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C3" s="111">
         <v>2.2584973866611409E-2</v>
       </c>
       <c r="D3" s="111" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="111" t="s">
         <v>111</v>
-      </c>
-      <c r="E3" s="111" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -2185,16 +2194,16 @@
         <v>90</v>
       </c>
       <c r="B4" s="132" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C4" s="132">
         <v>489.45</v>
       </c>
       <c r="D4" s="132" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E4" s="132" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F4" s="132"/>
       <c r="G4" s="132"/>
@@ -2229,10 +2238,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="41" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D1" s="41" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E1" s="41" t="s">
         <v>9</v>
@@ -2290,25 +2299,25 @@
         <v>29</v>
       </c>
       <c r="E1" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="I1" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="J1" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="K1" s="37" t="s">
         <v>119</v>
-      </c>
-      <c r="F1" s="38" t="s">
-        <v>120</v>
-      </c>
-      <c r="G1" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1" s="37" t="s">
-        <v>122</v>
-      </c>
-      <c r="I1" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="J1" s="38" t="s">
-        <v>124</v>
-      </c>
-      <c r="K1" s="37" t="s">
-        <v>125</v>
       </c>
       <c r="L1" s="37" t="s">
         <v>36</v>
@@ -2326,10 +2335,10 @@
     </row>
     <row r="2" spans="1:15 1029:1029" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="135" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B2" s="135" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C2" s="135"/>
       <c r="D2" s="135" t="s">
@@ -2337,7 +2346,7 @@
       </c>
       <c r="E2" s="135"/>
       <c r="F2" s="135" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="G2" s="135" t="b">
         <v>0</v>
@@ -2348,7 +2357,7 @@
       <c r="I2" s="135"/>
       <c r="J2" s="135"/>
       <c r="K2" s="135" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="L2" s="135"/>
       <c r="M2" s="135"/>
@@ -2356,7 +2365,7 @@
         <v>72</v>
       </c>
       <c r="O2" s="135" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="AMO2" s="135"/>
     </row>
@@ -2393,16 +2402,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C1" s="21" t="s">
         <v>33</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F1" s="21" t="s">
         <v>9</v>
@@ -2455,10 +2464,10 @@
         <v>54</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F1" s="35" t="s">
         <v>36</v>
@@ -2475,17 +2484,17 @@
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="137" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B2" s="137" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C2" s="137"/>
       <c r="D2" s="137">
         <v>2</v>
       </c>
       <c r="E2" s="137" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2498,7 +2507,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2515,22 +2524,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="H1" s="25" t="s">
         <v>13</v>
@@ -2553,16 +2562,16 @@
         <v>53</v>
       </c>
       <c r="D2" s="94" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E2" s="94">
         <v>1</v>
       </c>
       <c r="F2" s="94" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G2" s="94" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="H2" s="93"/>
       <c r="I2" s="93"/>
@@ -2570,7 +2579,7 @@
     </row>
     <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="100" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B3" s="101" t="s">
         <v>10</v>
@@ -2579,16 +2588,16 @@
         <v>87</v>
       </c>
       <c r="D3" s="101" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E3" s="101">
-        <v>992.98255190377824</v>
+        <v>992.98255190377802</v>
       </c>
       <c r="F3" s="101" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G3" s="101" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="H3" s="100"/>
       <c r="I3" s="100"/>
@@ -2596,7 +2605,7 @@
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="109" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B4" s="110" t="s">
         <v>10</v>
@@ -2605,26 +2614,26 @@
         <v>87</v>
       </c>
       <c r="D4" s="110" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E4" s="110">
         <v>489.45</v>
       </c>
       <c r="F4" s="110" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G4" s="110" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="H4" s="109"/>
       <c r="I4" s="109"/>
       <c r="J4" s="109" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="112" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B5" s="113" t="s">
         <v>10</v>
@@ -2633,7 +2642,7 @@
         <v>87</v>
       </c>
       <c r="D5" s="113" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E5" s="113">
         <v>5.5313109099319684</v>
@@ -2642,7 +2651,7 @@
         <v>91</v>
       </c>
       <c r="G5" s="113" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="H5" s="112"/>
       <c r="I5" s="112"/>
@@ -2650,7 +2659,7 @@
     </row>
     <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="126" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B6" s="127" t="s">
         <v>10</v>
@@ -2665,10 +2674,10 @@
         <v>0</v>
       </c>
       <c r="F6" s="127" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G6" s="127" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="H6" s="126"/>
       <c r="I6" s="126"/>
@@ -2676,7 +2685,7 @@
     </row>
     <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="126" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B7" s="127" t="s">
         <v>10</v>
@@ -2685,26 +2694,26 @@
         <v>67</v>
       </c>
       <c r="D7" s="127" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E7" s="127">
         <v>4.2500000000000003E-2</v>
       </c>
       <c r="F7" s="127" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G7" s="127" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="H7" s="126"/>
       <c r="I7" s="126"/>
       <c r="J7" s="126" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="130" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B8" s="131" t="s">
         <v>10</v>
@@ -2713,16 +2722,16 @@
         <v>74</v>
       </c>
       <c r="D8" s="131" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="E8" s="131">
         <v>4.8828698208797903</v>
       </c>
       <c r="F8" s="131" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G8" s="131" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="H8" s="130"/>
       <c r="I8" s="130"/>
@@ -2730,7 +2739,7 @@
     </row>
     <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="133" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B9" s="134" t="s">
         <v>10</v>
@@ -2739,16 +2748,16 @@
         <v>74</v>
       </c>
       <c r="D9" s="134" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E9" s="134">
         <v>2.2584973866611409E-2</v>
       </c>
       <c r="F9" s="134" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G9" s="134" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="H9" s="133"/>
       <c r="I9" s="133"/>
@@ -2788,31 +2797,31 @@
         <v>94</v>
       </c>
       <c r="B1" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="I1" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="J1" s="34" t="s">
         <v>154</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>155</v>
-      </c>
-      <c r="E1" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="F1" s="34" t="s">
-        <v>156</v>
-      </c>
-      <c r="G1" s="34" t="s">
-        <v>157</v>
-      </c>
-      <c r="H1" s="34" t="s">
-        <v>158</v>
-      </c>
-      <c r="I1" s="34" t="s">
-        <v>159</v>
-      </c>
-      <c r="J1" s="34" t="s">
-        <v>160</v>
       </c>
       <c r="K1" s="34" t="s">
         <v>13</v>
@@ -2826,25 +2835,25 @@
     </row>
     <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="138" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B2" s="138"/>
       <c r="C2" s="138"/>
       <c r="D2" s="138"/>
       <c r="E2" s="138" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F2" s="140" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G2" s="140" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H2" s="140">
         <v>37</v>
       </c>
       <c r="I2" s="139" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="J2" s="138"/>
       <c r="K2" s="138"/>
@@ -2855,25 +2864,25 @@
     </row>
     <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="138" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B3" s="138"/>
       <c r="C3" s="138"/>
       <c r="D3" s="138"/>
       <c r="E3" s="138" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F3" s="140" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G3" s="140" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H3" s="140">
         <v>37</v>
       </c>
       <c r="I3" s="140" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="J3" s="138"/>
       <c r="K3" s="138"/>
@@ -2881,50 +2890,50 @@
         <v>41</v>
       </c>
       <c r="M3" s="138" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="138" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B4" s="138"/>
       <c r="C4" s="138"/>
       <c r="D4" s="138"/>
       <c r="E4" s="138" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F4" s="140" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G4" s="140" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H4" s="140">
         <v>37</v>
       </c>
       <c r="I4" s="140" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="J4" s="138"/>
       <c r="K4" s="138"/>
       <c r="L4" s="138" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="M4" s="138"/>
     </row>
     <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="138" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B5" s="138"/>
       <c r="C5" s="138"/>
       <c r="D5" s="138"/>
       <c r="E5" s="138" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F5" s="140" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G5" s="138"/>
       <c r="H5" s="138"/>
@@ -2932,22 +2941,22 @@
       <c r="J5" s="138"/>
       <c r="K5" s="138"/>
       <c r="L5" s="138" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="M5" s="138"/>
     </row>
     <row r="6" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="141" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B6" s="141"/>
       <c r="C6" s="141"/>
       <c r="D6" s="141"/>
       <c r="E6" s="141" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F6" s="142" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G6" s="141"/>
       <c r="H6" s="141"/>
@@ -2955,36 +2964,36 @@
       <c r="J6" s="141"/>
       <c r="K6" s="141"/>
       <c r="L6" s="141" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="M6" s="141"/>
     </row>
     <row r="7" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="143" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B7" s="143"/>
       <c r="C7" s="143"/>
       <c r="D7" s="143"/>
       <c r="E7" s="143" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F7" s="145" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G7" s="145" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H7" s="144">
         <v>37</v>
       </c>
       <c r="I7" s="145" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="J7" s="143"/>
       <c r="K7" s="143"/>
       <c r="L7" s="143" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -3026,7 +3035,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3039,7 +3048,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="65" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -3081,25 +3090,25 @@
         <v>29</v>
       </c>
       <c r="D1" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="J1" s="21" t="s">
         <v>171</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="G1" s="29" t="s">
-        <v>174</v>
-      </c>
-      <c r="H1" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>176</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>177</v>
       </c>
       <c r="K1" s="25" t="s">
         <v>13</v>
@@ -3110,22 +3119,22 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="92" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B2" s="92" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C2" s="92" t="s">
+        <v>172</v>
+      </c>
+      <c r="D2" s="92" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="92" t="s">
-        <v>184</v>
-      </c>
       <c r="E2" s="92" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F2" s="92" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="G2" s="92">
         <v>326</v>
@@ -3134,13 +3143,13 @@
         <v>5957</v>
       </c>
       <c r="I2" s="92" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="J2" s="92">
         <v>2009</v>
       </c>
       <c r="K2" s="92" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -3148,19 +3157,19 @@
         <v>72</v>
       </c>
       <c r="B3" s="91" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C3" s="91" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D3" s="91" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="E3" s="91" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="F3" s="91" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="G3" s="91">
         <v>231</v>
@@ -3169,13 +3178,13 @@
         <v>1</v>
       </c>
       <c r="I3" s="91" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="J3" s="91">
         <v>1990</v>
       </c>
       <c r="K3" s="91" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -3183,13 +3192,13 @@
         <v>41</v>
       </c>
       <c r="B4" s="136" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="C4" s="136" t="s">
         <v>66</v>
       </c>
       <c r="D4" s="136" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E4" s="136"/>
       <c r="F4" s="136"/>
@@ -3203,22 +3212,22 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="146" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B5" s="146" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C5" s="146" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D5" s="146" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="E5" s="146" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="F5" s="146" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G5" s="146">
         <v>5</v>
@@ -3227,33 +3236,33 @@
         <v>12</v>
       </c>
       <c r="I5" s="146" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="J5" s="146">
         <v>2006</v>
       </c>
       <c r="K5" s="146" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="147" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B6" s="147" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C6" s="147" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D6" s="147" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="E6" s="147" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="F6" s="147" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="G6" s="147">
         <v>7</v>
@@ -3266,24 +3275,24 @@
         <v>2011</v>
       </c>
       <c r="K6" s="147" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="148" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B7" s="148" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C7" s="148" t="s">
         <v>66</v>
       </c>
       <c r="D7" s="148" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="E7" s="148" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="F7" s="148"/>
       <c r="G7" s="148"/>
@@ -3296,19 +3305,19 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="149" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B8" s="149" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C8" s="149" t="s">
         <v>66</v>
       </c>
       <c r="D8" s="149" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="E8" s="149" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="F8" s="149"/>
       <c r="G8" s="149"/>
@@ -3408,7 +3417,7 @@
   <dimension ref="A1:I776"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>